<commit_message>
refs #649 Passantenanalyse dokumentiert
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Passantenanalyse_Auswertung.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/03_Vorstudie/Passantenanalyse_Auswertung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15315" windowHeight="12075" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15315" windowHeight="6660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gesammelte Daten" sheetId="1" r:id="rId1"/>
@@ -759,6 +759,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1039,11 +1040,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104983168"/>
-        <c:axId val="107774336"/>
+        <c:axId val="106818176"/>
+        <c:axId val="106922368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104983168"/>
+        <c:axId val="106818176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1052,7 +1053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107774336"/>
+        <c:crossAx val="106922368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1060,7 +1061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107774336"/>
+        <c:axId val="106922368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,13 +1072,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104983168"/>
+        <c:crossAx val="106818176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1220,11 +1222,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108282624"/>
-        <c:axId val="108284544"/>
+        <c:axId val="107700992"/>
+        <c:axId val="107702912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108282624"/>
+        <c:axId val="107700992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1246,12 +1248,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108284544"/>
+        <c:crossAx val="107702912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1259,7 +1262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108284544"/>
+        <c:axId val="107702912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,7 +1273,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108282624"/>
+        <c:crossAx val="107700992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1446,11 +1449,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108530688"/>
-        <c:axId val="108545152"/>
+        <c:axId val="107949056"/>
+        <c:axId val="107959424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108530688"/>
+        <c:axId val="107949056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1481,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108545152"/>
+        <c:crossAx val="107959424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +1489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108545152"/>
+        <c:axId val="107959424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,7 +1500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108530688"/>
+        <c:crossAx val="107949056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8798,10 +8801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9174,6 +9177,12 @@
       <c r="B46">
         <f>SUMIF('Gesammelte Daten'!$B$2:$B$549,A46,'Gesammelte Daten'!$C$2:$C$549)</f>
         <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f>SUM(B2:B46)</f>
+        <v>1512</v>
       </c>
     </row>
   </sheetData>
@@ -9188,7 +9197,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="A2" sqref="A2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18833,7 +18842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
@@ -18934,7 +18943,7 @@
         <v>4</v>
       </c>
       <c r="K3">
-        <f>SUMIF($G$3:$G$277, J3, $D$3:$D$277)</f>
+        <f t="shared" ref="K3:K11" si="0">SUMIF($G$3:$G$277, J3, $D$3:$D$277)</f>
         <v>112</v>
       </c>
       <c r="L3" s="8">
@@ -18945,7 +18954,7 @@
         <v>5</v>
       </c>
       <c r="N3">
-        <f>SUMIF($H$3:$H$277, M3,$D$3:$D$277)</f>
+        <f t="shared" ref="N3:N11" si="1">SUMIF($H$3:$H$277, M3,$D$3:$D$277)</f>
         <v>86</v>
       </c>
       <c r="O3" s="8">
@@ -18985,26 +18994,26 @@
         <v>3</v>
       </c>
       <c r="K4">
-        <f>SUMIF($G$3:$G$277, J4, $D$3:$D$277)</f>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="L4" s="8">
-        <f t="shared" ref="L4:L11" si="0">(K4/SUM($K$3:$K$11))</f>
+        <f t="shared" ref="L4:L11" si="2">(K4/SUM($K$3:$K$11))</f>
         <v>0.2690909090909091</v>
       </c>
       <c r="M4" s="7">
         <v>4</v>
       </c>
       <c r="N4">
-        <f>SUMIF($H$3:$H$277, M4,$D$3:$D$277)</f>
+        <f t="shared" si="1"/>
         <v>79</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O11" si="1">(N4/SUM($N$3:$N$11))</f>
+        <f t="shared" ref="O4:O11" si="3">(N4/SUM($N$3:$N$11))</f>
         <v>0.28727272727272729</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" ref="P4:P11" si="2">((L4+O4)/2)</f>
+        <f t="shared" ref="P4:P11" si="4">((L4+O4)/2)</f>
         <v>0.2781818181818182</v>
       </c>
     </row>
@@ -19036,26 +19045,26 @@
         <v>5</v>
       </c>
       <c r="K5">
-        <f>SUMIF($G$3:$G$277, J5, $D$3:$D$277)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="L5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.15272727272727274</v>
       </c>
       <c r="M5" s="7">
         <v>6</v>
       </c>
       <c r="N5">
-        <f>SUMIF($H$3:$H$277, M5,$D$3:$D$277)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15636363636363637</v>
       </c>
     </row>
@@ -19087,26 +19096,26 @@
         <v>2</v>
       </c>
       <c r="K6">
-        <f>SUMIF($G$3:$G$277, J6, $D$3:$D$277)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="L6" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.3636363636363634E-2</v>
       </c>
       <c r="M6" s="7">
         <v>3</v>
       </c>
       <c r="N6">
-        <f>SUMIF($H$3:$H$277, M6,$D$3:$D$277)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="O6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.12727272727272726</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.10545454545454544</v>
       </c>
     </row>
@@ -19138,26 +19147,26 @@
         <v>6</v>
       </c>
       <c r="K7">
-        <f>SUMIF($G$3:$G$277, J7, $D$3:$D$277)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="L7" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.545454545454546E-2</v>
       </c>
       <c r="M7" s="7">
         <v>7</v>
       </c>
       <c r="N7">
-        <f>SUMIF($H$3:$H$277, M7,$D$3:$D$277)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="O7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.4545454545454543E-2</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.06</v>
       </c>
     </row>
@@ -19189,26 +19198,26 @@
         <v>8</v>
       </c>
       <c r="K8">
-        <f>SUMIF($G$3:$G$277, J8, $D$3:$D$277)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.090909090909091E-2</v>
       </c>
       <c r="M8" s="7">
         <v>8</v>
       </c>
       <c r="N8">
-        <f>SUMIF($H$3:$H$277, M8,$D$3:$D$277)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.272727272727273E-2</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.181818181818182E-2</v>
       </c>
     </row>
@@ -19240,26 +19249,26 @@
         <v>7</v>
       </c>
       <c r="K9">
-        <f>SUMIF($G$3:$G$277, J9, $D$3:$D$277)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L9" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.2727272727272727E-3</v>
       </c>
       <c r="M9" s="7">
         <v>2</v>
       </c>
       <c r="N9">
-        <f>SUMIF($H$3:$H$277, M9,$D$3:$D$277)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="O9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5454545454545455E-2</v>
       </c>
       <c r="P9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6363636363636365E-2</v>
       </c>
     </row>
@@ -19291,26 +19300,26 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f>SUMIF($G$3:$G$277, J10, $D$3:$D$277)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L10" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6363636363636364E-3</v>
       </c>
       <c r="M10" s="7">
         <v>1</v>
       </c>
       <c r="N10">
-        <f>SUMIF($H$3:$H$277, M10,$D$3:$D$277)</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="O10" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="P10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.8181818181818182E-3</v>
       </c>
     </row>
@@ -19342,26 +19351,26 @@
         <v>9</v>
       </c>
       <c r="K11">
-        <f>SUMIF($G$3:$G$277, J11, $D$3:$D$277)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="M11" s="7">
         <v>9</v>
       </c>
       <c r="N11">
-        <f>SUMIF($H$3:$H$277, M11,$D$3:$D$277)</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="O11" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="P11" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>